<commit_message>
Included hallucination into report
</commit_message>
<xml_diff>
--- a/output/support/scores.xlsx
+++ b/output/support/scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,1402 +457,954 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2318</v>
+        <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>20.9372</v>
+        <v>8.022166666666667</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.8284770449002584</v>
       </c>
       <c r="D2" t="n">
-        <v>10.4686</v>
+        <v>4.284534947831056</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>371</v>
+        <v>31</v>
       </c>
       <c r="B3" t="n">
-        <v>19.3074</v>
+        <v>6.799616666666666</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.4147921055555344</v>
       </c>
       <c r="D3" t="n">
-        <v>9.653700000000001</v>
+        <v>3.75321714727612</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1074</v>
+        <v>30</v>
       </c>
       <c r="B4" t="n">
-        <v>17.9203</v>
+        <v>7.471133333333333</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>8.960150000000001</v>
+        <v>3.735566666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1690</v>
+        <v>22</v>
       </c>
       <c r="B5" t="n">
-        <v>17.89051666666667</v>
+        <v>7.249383333333333</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>8.945258333333333</v>
+        <v>3.624691666666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>779</v>
+        <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>17.7746</v>
+        <v>5.6605</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.6776693363984426</v>
       </c>
       <c r="D6" t="n">
-        <v>8.8873</v>
+        <v>3.128282508046777</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1718</v>
+        <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>17.67</v>
+        <v>4.64</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.4245564788579941</v>
       </c>
       <c r="D7" t="n">
-        <v>8.835000000000001</v>
+        <v>2.670986435020694</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2006</v>
+        <v>68</v>
       </c>
       <c r="B8" t="n">
-        <v>17.4389</v>
+        <v>5.315383333333333</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>8.71945</v>
+        <v>2.657691666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2268</v>
+        <v>28</v>
       </c>
       <c r="B9" t="n">
-        <v>17.3399</v>
+        <v>3.7451</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.1000200305134058</v>
       </c>
       <c r="D9" t="n">
-        <v>8.66995</v>
+        <v>2.327087177624518</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>568</v>
+        <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>16.6778</v>
+        <v>3.981</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.8498266537984213</v>
       </c>
       <c r="D10" t="n">
-        <v>8.338900000000001</v>
+        <v>2.26079559714328</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1065</v>
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>16.3458</v>
+        <v>3.3615</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.07929091155529022</v>
       </c>
       <c r="D11" t="n">
-        <v>8.1729</v>
+        <v>2.144017127191394</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>489</v>
+        <v>6</v>
       </c>
       <c r="B12" t="n">
-        <v>16.2456</v>
+        <v>4.249133333333333</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>8.1228</v>
+        <v>2.124566666666666</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>468</v>
+        <v>41</v>
       </c>
       <c r="B13" t="n">
-        <v>16.1287</v>
+        <v>3.51365</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.5331113934516907</v>
       </c>
       <c r="D13" t="n">
-        <v>8.064349999999999</v>
+        <v>2.082959162289594</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>426</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>16.1238</v>
+        <v>3.430416666666666</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.6693164308865865</v>
       </c>
       <c r="D14" t="n">
-        <v>8.0619</v>
+        <v>2.014732132865125</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1873</v>
+        <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>16.0601</v>
+        <v>3.292783333333334</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>0.5737322171529134</v>
       </c>
       <c r="D15" t="n">
-        <v>8.030049999999999</v>
+        <v>1.964107726966027</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2385</v>
+        <v>65</v>
       </c>
       <c r="B16" t="n">
-        <v>16.0498</v>
+        <v>3.18455</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.574103112022082</v>
       </c>
       <c r="D16" t="n">
-        <v>8.024900000000001</v>
+        <v>1.909916199093815</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>369</v>
+        <v>4</v>
       </c>
       <c r="B17" t="n">
-        <v>15.9555</v>
+        <v>3.208583333333333</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.8045039375623068</v>
       </c>
       <c r="D17" t="n">
-        <v>7.97775</v>
+        <v>1.881376127161359</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="B18" t="n">
-        <v>15.7408</v>
+        <v>2.9361</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.3453667958577474</v>
       </c>
       <c r="D18" t="n">
-        <v>7.8704</v>
+        <v>1.839695860102577</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1687</v>
+        <v>63</v>
       </c>
       <c r="B19" t="n">
-        <v>15.6831</v>
+        <v>3.027666666666667</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>0.8617199460665385</v>
       </c>
       <c r="D19" t="n">
-        <v>7.84155</v>
+        <v>1.782402191424157</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2322</v>
+        <v>71</v>
       </c>
       <c r="B20" t="n">
-        <v>15.6708</v>
+        <v>2.965133333333334</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.8469143509864807</v>
       </c>
       <c r="D20" t="n">
-        <v>7.8354</v>
+        <v>1.753288478824842</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2092</v>
+        <v>70</v>
       </c>
       <c r="B21" t="n">
-        <v>15.6128</v>
+        <v>3.487633333333333</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>7.8064</v>
+        <v>1.743816666666667</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1543</v>
+        <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>15.5655</v>
+        <v>2.694816666666667</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>0.2692558070023854</v>
       </c>
       <c r="D22" t="n">
-        <v>7.78275</v>
+        <v>1.741339956290297</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2608</v>
+        <v>40</v>
       </c>
       <c r="B23" t="n">
-        <v>15.5655</v>
+        <v>2.557133333333333</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.385399396220843</v>
       </c>
       <c r="D23" t="n">
-        <v>7.78275</v>
+        <v>1.639473421328119</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2082</v>
+        <v>21</v>
       </c>
       <c r="B24" t="n">
-        <v>15.4628</v>
+        <v>2.3071</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.1718415965636571</v>
       </c>
       <c r="D24" t="n">
-        <v>7.7314</v>
+        <v>1.580228828833364</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2085</v>
+        <v>44</v>
       </c>
       <c r="B25" t="n">
-        <v>15.4545</v>
+        <v>3.151433333333333</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>7.72725</v>
+        <v>1.575716666666667</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1609</v>
+        <v>49</v>
       </c>
       <c r="B26" t="n">
-        <v>15.3426</v>
+        <v>3.148366666666667</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>7.6713</v>
+        <v>1.574183333333333</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2118</v>
+        <v>20</v>
       </c>
       <c r="B27" t="n">
-        <v>15.3157</v>
+        <v>3.11325</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>7.65785</v>
+        <v>1.556625</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2314</v>
+        <v>56</v>
       </c>
       <c r="B28" t="n">
-        <v>14.8523</v>
+        <v>2.323616666666667</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.6078332463900248</v>
       </c>
       <c r="D28" t="n">
-        <v>7.42615</v>
+        <v>1.472785856109791</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2000</v>
+        <v>16</v>
       </c>
       <c r="B29" t="n">
-        <v>14.8251</v>
+        <v>2.2489</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>0.4831327696641286</v>
       </c>
       <c r="D29" t="n">
-        <v>7.41255</v>
+        <v>1.461574234746179</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2026</v>
+        <v>42</v>
       </c>
       <c r="B30" t="n">
-        <v>14.7691</v>
+        <v>2.28276</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>0.6823876897493998</v>
       </c>
       <c r="D30" t="n">
-        <v>7.38455</v>
+        <v>1.438576658681257</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2083</v>
+        <v>54</v>
       </c>
       <c r="B31" t="n">
-        <v>14.39025</v>
+        <v>2.1557</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>0.4074766536553701</v>
       </c>
       <c r="D31" t="n">
-        <v>7.195125</v>
+        <v>1.433095679352084</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>994</v>
+        <v>23</v>
       </c>
       <c r="B32" t="n">
-        <v>14.3492</v>
+        <v>2.807266666666667</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>7.1746</v>
+        <v>1.403633333333334</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2330</v>
+        <v>17</v>
       </c>
       <c r="B33" t="n">
-        <v>13.96845</v>
+        <v>2.21276</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>0.6875815490881602</v>
       </c>
       <c r="D33" t="n">
-        <v>6.984225</v>
+        <v>1.402661978355453</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2203</v>
+        <v>55</v>
       </c>
       <c r="B34" t="n">
-        <v>13.708725</v>
+        <v>2.0852</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>0.5522183477878571</v>
       </c>
       <c r="D34" t="n">
-        <v>6.8543625</v>
+        <v>1.36471963008463</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2205</v>
+        <v>48</v>
       </c>
       <c r="B35" t="n">
-        <v>13.57625</v>
+        <v>2.047633333333333</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>0.5522995193799337</v>
       </c>
       <c r="D35" t="n">
-        <v>6.788125</v>
+        <v>1.3459194527319</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1048</v>
+        <v>29</v>
       </c>
       <c r="B36" t="n">
-        <v>13.57275</v>
+        <v>1.5768</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.2729939917723338</v>
       </c>
       <c r="D36" t="n">
-        <v>6.786375</v>
+        <v>1.181174831013831</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2381</v>
+        <v>25</v>
       </c>
       <c r="B37" t="n">
-        <v>13.50623333333333</v>
+        <v>2.310933333333333</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6.753116666666667</v>
+        <v>1.155466666666667</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>933</v>
+        <v>18</v>
       </c>
       <c r="B38" t="n">
-        <v>13.48843333333333</v>
+        <v>2.2476</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6.744216666666667</v>
+        <v>1.1238</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2383</v>
+        <v>43</v>
       </c>
       <c r="B39" t="n">
-        <v>13.2136</v>
+        <v>1.556416666666667</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>0.4869122405846913</v>
       </c>
       <c r="D39" t="n">
-        <v>6.6068</v>
+        <v>1.114475657222864</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1675</v>
+        <v>24</v>
       </c>
       <c r="B40" t="n">
-        <v>13.21092</v>
+        <v>2.0974</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.605460000000001</v>
+        <v>1.0487</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1671</v>
+        <v>36</v>
       </c>
       <c r="B41" t="n">
-        <v>13.17176</v>
+        <v>1.3551</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>0.3483638912439346</v>
       </c>
       <c r="D41" t="n">
-        <v>6.58588</v>
+        <v>1.048369778879368</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1625</v>
+        <v>33</v>
       </c>
       <c r="B42" t="n">
-        <v>13.0584</v>
+        <v>1.49125</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>0.7269851267337799</v>
       </c>
       <c r="D42" t="n">
-        <v>6.5292</v>
+        <v>1.035146891219551</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2380</v>
+        <v>12</v>
       </c>
       <c r="B43" t="n">
-        <v>12.99874</v>
+        <v>1.923566666666667</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6.499370000000001</v>
+        <v>0.9617833333333334</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>901</v>
+        <v>35</v>
       </c>
       <c r="B44" t="n">
-        <v>12.83178333333333</v>
+        <v>1.098033333333333</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>0.2874728838602702</v>
       </c>
       <c r="D44" t="n">
-        <v>6.415891666666667</v>
+        <v>0.9373743604619988</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2105</v>
+        <v>50</v>
       </c>
       <c r="B45" t="n">
-        <v>12.5829</v>
+        <v>1.1866</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>0.7322065234184265</v>
       </c>
       <c r="D45" t="n">
-        <v>6.291449999999999</v>
+        <v>0.8819491842862213</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>525</v>
+        <v>7</v>
       </c>
       <c r="B46" t="n">
-        <v>12.42604</v>
+        <v>1.64225</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6.21302</v>
+        <v>0.821125</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1666</v>
+        <v>27</v>
       </c>
       <c r="B47" t="n">
-        <v>12.240475</v>
+        <v>1.528333333333333</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6.1202375</v>
+        <v>0.7641666666666667</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1043</v>
+        <v>26</v>
       </c>
       <c r="B48" t="n">
-        <v>12.0673</v>
+        <v>1.361</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6.03365</v>
+        <v>0.6805</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2378</v>
+        <v>37</v>
       </c>
       <c r="B49" t="n">
-        <v>12.018575</v>
+        <v>0.73982</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>0.6359184881051382</v>
       </c>
       <c r="D49" t="n">
-        <v>6.0092875</v>
+        <v>0.6755486999936305</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1326</v>
+        <v>8</v>
       </c>
       <c r="B50" t="n">
-        <v>11.54228333333333</v>
+        <v>1.248</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>5.771141666666666</v>
+        <v>0.624</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1679</v>
+        <v>45</v>
       </c>
       <c r="B51" t="n">
-        <v>11.4667</v>
+        <v>0.818375</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>5.733350000000001</v>
+        <v>0.4091875</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>563</v>
+        <v>11</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9130187034606934</v>
+        <v>0.4709108124176661</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2613670211877641</v>
+        <v>0.3399254365247161</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1363</v>
+        <v>66</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9133754968643188</v>
+        <v>0.5001017252604166</v>
       </c>
       <c r="D53" t="n">
-        <v>0.261318283222196</v>
+        <v>0.3333107292528448</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1365</v>
+        <v>57</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9142987728118896</v>
+        <v>0.5334753592809042</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2611922480969657</v>
+        <v>0.3260567553132813</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2361</v>
+        <v>58</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9151636362075806</v>
+        <v>0.5563210447629293</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2610742970193937</v>
+        <v>0.3212704741624591</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>275</v>
+        <v>34</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.9180551767349243</v>
+        <v>0.5638064841429392</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2606807176689996</v>
+        <v>0.3197326555875168</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>363</v>
+        <v>62</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9181689620018005</v>
+        <v>0.5644363810618719</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2606652541589455</v>
+        <v>0.3196039200140702</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>649</v>
+        <v>59</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9193505048751831</v>
+        <v>0.5704296181599299</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2605047898911593</v>
+        <v>0.3183842142418641</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>367</v>
+        <v>64</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9244180917739868</v>
+        <v>0.571307455499967</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2598188003621837</v>
+        <v>0.3182063435452276</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>743</v>
+        <v>39</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.925784707069397</v>
+        <v>0.6477482616901398</v>
       </c>
       <c r="D60" t="n">
-        <v>0.259634422354971</v>
+        <v>0.3034444105479659</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1089</v>
+        <v>67</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9277659257253011</v>
+        <v>0.6818446715672811</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2593675888382976</v>
+        <v>0.2972926147419184</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2272</v>
+        <v>38</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9281411170959473</v>
+        <v>0.6864465673764547</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2593171192537352</v>
+        <v>0.2964813766841319</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1831</v>
+        <v>14</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9291470050811768</v>
+        <v>0.7058454155921936</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2591819071760996</v>
+        <v>0.2931097949613578</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>737</v>
+        <v>61</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9306689500808716</v>
+        <v>0.7059069772561392</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2589775942577085</v>
+        <v>0.293099217405291</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>920</v>
+        <v>53</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.9323745965957642</v>
+        <v>0.7211113572120667</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2587490028490556</v>
+        <v>0.2905099649158799</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>410</v>
+        <v>51</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9326578974723816</v>
+        <v>0.7369084258874258</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2587110738294257</v>
+        <v>0.2878677957616209</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1630</v>
+        <v>47</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9330296218395233</v>
+        <v>0.7638867497444153</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2586613233190842</v>
+        <v>0.2834649106993118</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>365</v>
+        <v>52</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9332654178142548</v>
+        <v>0.7739376227060953</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2586297749872849</v>
+        <v>0.2818588396796405</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1834</v>
+        <v>60</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.93342325091362</v>
+        <v>0.7855493525664011</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2586086620007957</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>146</v>
-      </c>
-      <c r="B70" t="n">
-        <v>0</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0.9335484206676483</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0.2585919207688378</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>1144</v>
-      </c>
-      <c r="B71" t="n">
-        <v>0</v>
-      </c>
-      <c r="C71" t="n">
-        <v>0.9343869388103485</v>
-      </c>
-      <c r="D71" t="n">
-        <v>0.2584798263306621</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>2134</v>
-      </c>
-      <c r="B72" t="n">
-        <v>0</v>
-      </c>
-      <c r="C72" t="n">
-        <v>0.9351553320884705</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0.2583771915923601</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>544</v>
-      </c>
-      <c r="B73" t="n">
-        <v>0</v>
-      </c>
-      <c r="C73" t="n">
-        <v>0.9353585362434387</v>
-      </c>
-      <c r="D73" t="n">
-        <v>0.2583500631208664</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>2403</v>
-      </c>
-      <c r="B74" t="n">
-        <v>0</v>
-      </c>
-      <c r="C74" t="n">
-        <v>0.9353830019632975</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0.2583467972451904</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>926</v>
-      </c>
-      <c r="B75" t="n">
-        <v>0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>0.9359023968378702</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.2582774838321947</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>1085</v>
-      </c>
-      <c r="B76" t="n">
-        <v>0</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0.9360684275627136</v>
-      </c>
-      <c r="D76" t="n">
-        <v>0.2582553348227687</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>1717</v>
-      </c>
-      <c r="B77" t="n">
-        <v>0</v>
-      </c>
-      <c r="C77" t="n">
-        <v>0.9361246824264526</v>
-      </c>
-      <c r="D77" t="n">
-        <v>0.2582478311124952</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>1207</v>
-      </c>
-      <c r="B78" t="n">
-        <v>0</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0.9362150430679321</v>
-      </c>
-      <c r="D78" t="n">
-        <v>0.258235779021606</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>408</v>
-      </c>
-      <c r="B79" t="n">
-        <v>0</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0.9380787491798401</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0.2579874528894097</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>1173</v>
-      </c>
-      <c r="B80" t="n">
-        <v>0</v>
-      </c>
-      <c r="C80" t="n">
-        <v>0.9381746153036753</v>
-      </c>
-      <c r="D80" t="n">
-        <v>0.2579746922965759</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>1300</v>
-      </c>
-      <c r="B81" t="n">
-        <v>0</v>
-      </c>
-      <c r="C81" t="n">
-        <v>0.9386717081069946</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0.2579085452731047</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>1172</v>
-      </c>
-      <c r="B82" t="n">
-        <v>0</v>
-      </c>
-      <c r="C82" t="n">
-        <v>0.9392014741897583</v>
-      </c>
-      <c r="D82" t="n">
-        <v>0.2578380878185497</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>667</v>
-      </c>
-      <c r="B83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C83" t="n">
-        <v>0.9396663427352905</v>
-      </c>
-      <c r="D83" t="n">
-        <v>0.2577762932643905</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>427</v>
-      </c>
-      <c r="B84" t="n">
-        <v>0</v>
-      </c>
-      <c r="C84" t="n">
-        <v>0.9397070050239563</v>
-      </c>
-      <c r="D84" t="n">
-        <v>0.2577708894719514</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>1721</v>
-      </c>
-      <c r="B85" t="n">
-        <v>0</v>
-      </c>
-      <c r="C85" t="n">
-        <v>0.939718770980835</v>
-      </c>
-      <c r="D85" t="n">
-        <v>0.2577693258838604</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>2197</v>
-      </c>
-      <c r="B86" t="n">
-        <v>0</v>
-      </c>
-      <c r="C86" t="n">
-        <v>0.9404446005821228</v>
-      </c>
-      <c r="D86" t="n">
-        <v>0.2576729064308266</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>1090</v>
-      </c>
-      <c r="B87" t="n">
-        <v>0</v>
-      </c>
-      <c r="C87" t="n">
-        <v>0.9407505293687185</v>
-      </c>
-      <c r="D87" t="n">
-        <v>0.2576322883511661</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>1263</v>
-      </c>
-      <c r="B88" t="n">
-        <v>0</v>
-      </c>
-      <c r="C88" t="n">
-        <v>0.9408249258995056</v>
-      </c>
-      <c r="D88" t="n">
-        <v>0.257622412680148</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>1538</v>
-      </c>
-      <c r="B89" t="n">
-        <v>0</v>
-      </c>
-      <c r="C89" t="n">
-        <v>0.9419366518656412</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0.2574749281958524</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>2603</v>
-      </c>
-      <c r="B90" t="n">
-        <v>0</v>
-      </c>
-      <c r="C90" t="n">
-        <v>0.9419366518656412</v>
-      </c>
-      <c r="D90" t="n">
-        <v>0.2574749281958524</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>1667</v>
-      </c>
-      <c r="B91" t="n">
-        <v>0</v>
-      </c>
-      <c r="C91" t="n">
-        <v>0.9420714477698008</v>
-      </c>
-      <c r="D91" t="n">
-        <v>0.2574570572952816</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>411</v>
-      </c>
-      <c r="B92" t="n">
-        <v>0</v>
-      </c>
-      <c r="C92" t="n">
-        <v>0.9421418408552805</v>
-      </c>
-      <c r="D92" t="n">
-        <v>0.2574477257437644</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>1504</v>
-      </c>
-      <c r="B93" t="n">
-        <v>0</v>
-      </c>
-      <c r="C93" t="n">
-        <v>0.9422391057014465</v>
-      </c>
-      <c r="D93" t="n">
-        <v>0.2574348330914814</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>2569</v>
-      </c>
-      <c r="B94" t="n">
-        <v>0</v>
-      </c>
-      <c r="C94" t="n">
-        <v>0.9422391057014465</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0.2574348330914814</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>482</v>
-      </c>
-      <c r="B95" t="n">
-        <v>0</v>
-      </c>
-      <c r="C95" t="n">
-        <v>0.9423869013786316</v>
-      </c>
-      <c r="D95" t="n">
-        <v>0.2574152449468843</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>1129</v>
-      </c>
-      <c r="B96" t="n">
-        <v>0</v>
-      </c>
-      <c r="C96" t="n">
-        <v>0.9430043598016103</v>
-      </c>
-      <c r="D96" t="n">
-        <v>0.2573334421396009</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>2060</v>
-      </c>
-      <c r="B97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C97" t="n">
-        <v>0.94405517578125</v>
-      </c>
-      <c r="D97" t="n">
-        <v>0.257194346245377</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>1171</v>
-      </c>
-      <c r="B98" t="n">
-        <v>0</v>
-      </c>
-      <c r="C98" t="n">
-        <v>0.9443459272384643</v>
-      </c>
-      <c r="D98" t="n">
-        <v>0.2571558862008393</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>2298</v>
-      </c>
-      <c r="B99" t="n">
-        <v>0</v>
-      </c>
-      <c r="C99" t="n">
-        <v>0.9449450016021729</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0.2570766780490547</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>90</v>
-      </c>
-      <c r="B100" t="n">
-        <v>0</v>
-      </c>
-      <c r="C100" t="n">
-        <v>0.9466014504432678</v>
-      </c>
-      <c r="D100" t="n">
-        <v>0.2568579201901566</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>691</v>
-      </c>
-      <c r="B101" t="n">
-        <v>0</v>
-      </c>
-      <c r="C101" t="n">
-        <v>0.9482581814130148</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0.2566394971519455</v>
+        <v>0.280025863906445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add gene data files and enhance debug logging
Added new gene data files to data/GSEA/external_gene_data, including gene_descriptions.csv, rat_genes_consolidated.txt.gz, and wikipathways_synonyms_Rattus_norvegicus.gmt(.gz). Updated RAG_workflow.py with extensive debug and status logging for file processing, embedding, and database checks to improve traceability and troubleshooting. Minor updates to .idea config files.
</commit_message>
<xml_diff>
--- a/output/support/scores.xlsx
+++ b/output/support/scores.xlsx
@@ -457,1402 +457,1402 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4275</v>
+        <v>8798</v>
       </c>
       <c r="B2" t="n">
-        <v>27.3664</v>
+        <v>24.8227</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>13.6832</v>
+        <v>12.41135</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1675</v>
+        <v>7038</v>
       </c>
       <c r="B3" t="n">
-        <v>27.3664</v>
+        <v>22.8009</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>13.6832</v>
+        <v>11.40045</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3649</v>
+        <v>3207</v>
       </c>
       <c r="B4" t="n">
-        <v>26.93073333333334</v>
+        <v>22.8009</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>13.46536666666667</v>
+        <v>11.40045</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1048</v>
+        <v>8050</v>
       </c>
       <c r="B5" t="n">
-        <v>26.93073333333334</v>
+        <v>22.8009</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>13.46536666666667</v>
+        <v>11.40045</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>371</v>
+        <v>9621</v>
       </c>
       <c r="B6" t="n">
-        <v>24.3742</v>
+        <v>22.8009</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>12.1871</v>
+        <v>11.40045</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4805</v>
+        <v>14202</v>
       </c>
       <c r="B7" t="n">
-        <v>22.9209</v>
+        <v>21.2276</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>11.46045</v>
+        <v>10.6138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2205</v>
+        <v>6734</v>
       </c>
       <c r="B8" t="n">
-        <v>22.9209</v>
+        <v>21.2276</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>11.46045</v>
+        <v>10.6138</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4803</v>
+        <v>8731</v>
       </c>
       <c r="B9" t="n">
-        <v>21.332</v>
+        <v>21.2276</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>10.666</v>
+        <v>10.6138</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2203</v>
+        <v>1185</v>
       </c>
       <c r="B10" t="n">
-        <v>21.332</v>
+        <v>21.2276</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>10.666</v>
+        <v>10.6138</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3115</v>
+        <v>5216</v>
       </c>
       <c r="B11" t="n">
-        <v>21.1247</v>
+        <v>19.8573</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>10.56235</v>
+        <v>9.928649999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>447</v>
+        <v>21168</v>
       </c>
       <c r="B12" t="n">
-        <v>21.1247</v>
+        <v>19.8573</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>10.56235</v>
+        <v>9.928649999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2318</v>
+        <v>1408</v>
       </c>
       <c r="B13" t="n">
-        <v>21.0006</v>
+        <v>19.8573</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>10.5003</v>
+        <v>9.928649999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4918</v>
+        <v>2924</v>
       </c>
       <c r="B14" t="n">
-        <v>21.0006</v>
+        <v>18.6533</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>10.5003</v>
+        <v>9.326650000000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>369</v>
+        <v>2909</v>
       </c>
       <c r="B15" t="n">
-        <v>20.5907</v>
+        <v>18.6533</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>10.29535</v>
+        <v>9.326650000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2002</v>
+        <v>7485</v>
       </c>
       <c r="B16" t="n">
-        <v>20.4727</v>
+        <v>18.6533</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>10.23635</v>
+        <v>9.326650000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>4602</v>
+        <v>1506</v>
       </c>
       <c r="B17" t="n">
-        <v>20.4727</v>
+        <v>18.6533</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>10.23635</v>
+        <v>9.326650000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>500</v>
+        <v>781</v>
       </c>
       <c r="B18" t="n">
-        <v>19.9816</v>
+        <v>16.80278333333333</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>9.9908</v>
+        <v>8.401391666666667</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2093</v>
+        <v>3152</v>
       </c>
       <c r="B19" t="n">
-        <v>19.3031</v>
+        <v>15.9631</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>9.65155</v>
+        <v>7.981550000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>4981</v>
+        <v>10197</v>
       </c>
       <c r="B20" t="n">
-        <v>19.26123333333333</v>
+        <v>15.9631</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>9.630616666666667</v>
+        <v>7.981550000000001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2381</v>
+        <v>21975</v>
       </c>
       <c r="B21" t="n">
-        <v>19.26123333333333</v>
+        <v>15.9225</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>9.630616666666667</v>
+        <v>7.96125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>4683</v>
+        <v>23121</v>
       </c>
       <c r="B22" t="n">
-        <v>18.8846</v>
+        <v>15.9225</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>9.442299999999999</v>
+        <v>7.96125</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2083</v>
+        <v>21098</v>
       </c>
       <c r="B23" t="n">
-        <v>18.8846</v>
+        <v>15.3925</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>9.442299999999999</v>
+        <v>7.69625</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2378</v>
+        <v>12690</v>
       </c>
       <c r="B24" t="n">
-        <v>18.7059</v>
+        <v>14.7781</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>9.35295</v>
+        <v>7.38905</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4978</v>
+        <v>1008</v>
       </c>
       <c r="B25" t="n">
-        <v>18.7059</v>
+        <v>14.2776</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>9.35295</v>
+        <v>7.1388</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>426</v>
+        <v>18794</v>
       </c>
       <c r="B26" t="n">
-        <v>18.7045</v>
+        <v>13.8833</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>9.35225</v>
+        <v>6.94165</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>3094</v>
+        <v>7961</v>
       </c>
       <c r="B27" t="n">
-        <v>18.7045</v>
+        <v>13.8833</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>9.35225</v>
+        <v>6.94165</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>4640</v>
+        <v>22045</v>
       </c>
       <c r="B28" t="n">
-        <v>18.6444</v>
+        <v>13.5616</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>9.3222</v>
+        <v>6.7808</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2040</v>
+        <v>3376</v>
       </c>
       <c r="B29" t="n">
-        <v>18.6444</v>
+        <v>13.5616</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>9.3222</v>
+        <v>6.7808</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1625</v>
+        <v>16730</v>
       </c>
       <c r="B30" t="n">
-        <v>18.6334</v>
+        <v>13.5616</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>9.316700000000001</v>
+        <v>6.7808</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4225</v>
+        <v>4930</v>
       </c>
       <c r="B31" t="n">
-        <v>18.6334</v>
+        <v>13.5428</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>9.316700000000001</v>
+        <v>6.7714</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>468</v>
+        <v>7168</v>
       </c>
       <c r="B32" t="n">
-        <v>18.4593</v>
+        <v>13.3676</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>9.229649999999999</v>
+        <v>6.6838</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>3136</v>
+        <v>7930</v>
       </c>
       <c r="B33" t="n">
-        <v>18.4593</v>
+        <v>13.0587</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>9.229649999999999</v>
+        <v>6.52935</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>4279</v>
+        <v>9114</v>
       </c>
       <c r="B34" t="n">
-        <v>18.4218</v>
+        <v>12.8873</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>9.210900000000001</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1679</v>
+        <v>9525</v>
       </c>
       <c r="B35" t="n">
-        <v>18.4218</v>
+        <v>12.8873</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>9.210900000000001</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1690</v>
+        <v>4168</v>
       </c>
       <c r="B36" t="n">
-        <v>18.15023333333333</v>
+        <v>12.8873</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>9.075116666666666</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>4290</v>
+        <v>25631</v>
       </c>
       <c r="B37" t="n">
-        <v>18.15023333333333</v>
+        <v>12.8873</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>9.075116666666666</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>430</v>
+        <v>383</v>
       </c>
       <c r="B38" t="n">
-        <v>17.8826</v>
+        <v>12.8873</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>8.9413</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3098</v>
+        <v>17024</v>
       </c>
       <c r="B39" t="n">
-        <v>17.8826</v>
+        <v>12.8873</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>8.9413</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2385</v>
+        <v>14626</v>
       </c>
       <c r="B40" t="n">
-        <v>17.53163333333333</v>
+        <v>12.8873</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>8.765816666666666</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4985</v>
+        <v>11980</v>
       </c>
       <c r="B41" t="n">
-        <v>17.53163333333333</v>
+        <v>12.8873</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>8.765816666666666</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2330</v>
+        <v>7995</v>
       </c>
       <c r="B42" t="n">
-        <v>17.32635</v>
+        <v>12.8873</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>8.663174999999999</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4930</v>
+        <v>21226</v>
       </c>
       <c r="B43" t="n">
-        <v>17.32635</v>
+        <v>12.8873</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>8.663174999999999</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>933</v>
+        <v>9700</v>
       </c>
       <c r="B44" t="n">
-        <v>16.9155</v>
+        <v>12.8873</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>8.457749999999999</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>3534</v>
+        <v>19467</v>
       </c>
       <c r="B45" t="n">
-        <v>16.9155</v>
+        <v>12.8873</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>8.457749999999999</v>
+        <v>6.443650000000001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>526</v>
+        <v>17046</v>
       </c>
       <c r="B46" t="n">
-        <v>16.60765</v>
+        <v>12.8725</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>8.303825</v>
+        <v>6.43625</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>3502</v>
+        <v>13856</v>
       </c>
       <c r="B47" t="n">
-        <v>16.24638</v>
+        <v>12.2241</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>8.123189999999999</v>
+        <v>6.11205</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>901</v>
+        <v>13374</v>
       </c>
       <c r="B48" t="n">
-        <v>16.24638</v>
+        <v>12.2241</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>8.123189999999999</v>
+        <v>6.11205</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>4654</v>
+        <v>21436</v>
       </c>
       <c r="B49" t="n">
-        <v>16.19273333333333</v>
+        <v>12.091</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>8.096366666666666</v>
+        <v>6.0455</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>4864</v>
+        <v>2848</v>
       </c>
       <c r="B50" t="n">
-        <v>16.0502</v>
+        <v>12.091</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>8.0251</v>
+        <v>6.0455</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2264</v>
+        <v>18275</v>
       </c>
       <c r="B51" t="n">
-        <v>16.0502</v>
+        <v>12.0605</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>8.0251</v>
+        <v>6.03025</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>4734</v>
+        <v>12094</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.9436930418014526</v>
+        <v>0.8988950252532959</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2572422647233383</v>
+        <v>0.2633110273872588</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2134</v>
+        <v>315</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.9436931014060974</v>
+        <v>0.8995209634304047</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2572422568348328</v>
+        <v>0.2632242600245034</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1263</v>
+        <v>15965</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9447106719017029</v>
+        <v>0.9020004272460938</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2571076547397447</v>
+        <v>0.2628811186567134</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3864</v>
+        <v>18097</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9447107315063477</v>
+        <v>0.9020424783229828</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2571076468594928</v>
+        <v>0.2628753067811853</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>425</v>
+        <v>1974</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.9464291334152222</v>
+        <v>0.9023942947387695</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2568806597765496</v>
+        <v>0.2628266923333358</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3093</v>
+        <v>12756</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9464292228221893</v>
+        <v>0.9029656648635864</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2568806479770347</v>
+        <v>0.2627477779720436</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1667</v>
+        <v>17243</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9473365843296051</v>
+        <v>0.9031985998153687</v>
       </c>
       <c r="D58" t="n">
-        <v>0.256760954435687</v>
+        <v>0.2627156199297885</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>4267</v>
+        <v>14790</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9473366737365723</v>
+        <v>0.9039535522460938</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2567609426471665</v>
+        <v>0.2626114483781131</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2065</v>
+        <v>11250</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9494640231132507</v>
+        <v>0.9044677019119263</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2564807526950464</v>
+        <v>0.2625405510936425</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>4665</v>
+        <v>5203</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9494640827178955</v>
+        <v>0.9044732451438904</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2564807448531763</v>
+        <v>0.2625397869331701</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1207</v>
+        <v>10539</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9513188600540161</v>
+        <v>0.905234232544899</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2562369534962415</v>
+        <v>0.2624349234645704</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>3808</v>
+        <v>11860</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9513188600540161</v>
+        <v>0.9052505493164062</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2562369534962415</v>
+        <v>0.2624326759435379</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2403</v>
+        <v>14704</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.951763371626536</v>
+        <v>0.9056225717067719</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2561785958629382</v>
+        <v>0.2623814429067004</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>5003</v>
+        <v>17269</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.9517634709676107</v>
+        <v>0.906856432557106</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2561785828239315</v>
+        <v>0.2622116649492574</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>3773</v>
+        <v>13147</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9518952369689941</v>
+        <v>0.9072015881538391</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2561612890538256</v>
+        <v>0.2621642112221589</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1172</v>
+        <v>4455</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9518954157829285</v>
+        <v>0.9072189182043076</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2561612655867856</v>
+        <v>0.2621618290525148</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>3250</v>
+        <v>26999</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9519865314165751</v>
+        <v>0.9076013565063477</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2561493083854146</v>
+        <v>0.2621092705216559</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>649</v>
+        <v>5226</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.95198655128479</v>
+        <v>0.9076150059700012</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2561493057782093</v>
+        <v>0.2621073950641081</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1726</v>
+        <v>14251</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.9521504441897074</v>
+        <v>0.9079282283782959</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2561278007482351</v>
+        <v>0.2620643651910276</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>4326</v>
+        <v>13100</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9521505037943522</v>
+        <v>0.9079800844192505</v>
       </c>
       <c r="D71" t="n">
-        <v>0.256127792927933</v>
+        <v>0.2620572426740972</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>3079</v>
+        <v>3085</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9537118872006735</v>
+        <v>0.9084427356719971</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2559230986286378</v>
+        <v>0.2619937138558894</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>411</v>
+        <v>13442</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.9537118872006735</v>
+        <v>0.908580482006073</v>
       </c>
       <c r="D73" t="n">
-        <v>0.2559230986286378</v>
+        <v>0.261974805209398</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>175</v>
+        <v>16205</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9543171167373657</v>
+        <v>0.9086835086345673</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2558438421880708</v>
+        <v>0.2619606643731572</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2846</v>
+        <v>21782</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9543171167373657</v>
+        <v>0.9090400040149689</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2558438421880708</v>
+        <v>0.2619117456671586</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>5170</v>
+        <v>14463</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9545172929763794</v>
+        <v>0.9099763184785843</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2558176393715041</v>
+        <v>0.2617833504858748</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>4105</v>
+        <v>4653</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9545172929763794</v>
+        <v>0.9101221164067587</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2558176393715041</v>
+        <v>0.2617633687947548</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1505</v>
+        <v>13638</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9545173645019531</v>
+        <v>0.9104804793993632</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2558176300098562</v>
+        <v>0.2617142678983013</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2570</v>
+        <v>15886</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9545173645019531</v>
+        <v>0.9106599092483521</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2558176300098562</v>
+        <v>0.2616896903419607</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>667</v>
+        <v>4961</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9548971652984619</v>
+        <v>0.9115528225898742</v>
       </c>
       <c r="D80" t="n">
-        <v>0.2557679293190151</v>
+        <v>0.2615674513888521</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>3268</v>
+        <v>5114</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9548973441123962</v>
+        <v>0.9117672840754191</v>
       </c>
       <c r="D81" t="n">
-        <v>0.2557679059239914</v>
+        <v>0.2615381088299213</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>174</v>
+        <v>17377</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9555246472358704</v>
+        <v>0.9118037819862366</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2556858593967347</v>
+        <v>0.2615331158517394</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2845</v>
+        <v>11873</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9555248260498047</v>
+        <v>0.9126194715499878</v>
       </c>
       <c r="D83" t="n">
-        <v>0.2556858360167225</v>
+        <v>0.2614215778085746</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1129</v>
+        <v>16130</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.9555587768554688</v>
+        <v>0.9132238427797953</v>
       </c>
       <c r="D84" t="n">
-        <v>0.2556813970091956</v>
+        <v>0.2613389969432595</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>3730</v>
+        <v>1968</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9555588364601135</v>
+        <v>0.9138243198394775</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2556813892161297</v>
+        <v>0.2612569998284574</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>4138</v>
+        <v>29079</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9557410955429078</v>
+        <v>0.9138715147972107</v>
       </c>
       <c r="D86" t="n">
-        <v>0.255657561800736</v>
+        <v>0.2612505573828862</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>5203</v>
+        <v>7855</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9557410955429078</v>
+        <v>0.9144208331902822</v>
       </c>
       <c r="D87" t="n">
-        <v>0.255657561800736</v>
+        <v>0.2611755949013447</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2603</v>
+        <v>10524</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9557411074638367</v>
+        <v>0.9147552102804184</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2556575602424133</v>
+        <v>0.2611299853451107</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1538</v>
+        <v>13384</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9557411074638367</v>
+        <v>0.9150511920452118</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2556575602424133</v>
+        <v>0.2610896262600774</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>90</v>
+        <v>17256</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9562437534332275</v>
+        <v>0.9152307748794556</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2555918704519797</v>
+        <v>0.2610651450248704</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2761</v>
+        <v>13990</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9562437534332275</v>
+        <v>0.9154833257198334</v>
       </c>
       <c r="D91" t="n">
-        <v>0.2555918704519797</v>
+        <v>0.261030724353657</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1504</v>
+        <v>13782</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9573091765244802</v>
+        <v>0.9158063769340515</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2554527440002254</v>
+        <v>0.2609867082706823</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2569</v>
+        <v>15737</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9573091765244802</v>
+        <v>0.9161118268966675</v>
       </c>
       <c r="D93" t="n">
-        <v>0.2554527440002254</v>
+        <v>0.2609451040286095</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>5169</v>
+        <v>12204</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9573092659314474</v>
+        <v>0.9174277037382126</v>
       </c>
       <c r="D94" t="n">
-        <v>0.2554527323315252</v>
+        <v>0.2607660247242705</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>4104</v>
+        <v>15638</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9573092659314474</v>
+        <v>0.917534863948822</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2554527323315252</v>
+        <v>0.2607514519816025</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>4655</v>
+        <v>11256</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9573366403579712</v>
+        <v>0.9178102115790049</v>
       </c>
       <c r="D96" t="n">
-        <v>0.2554491596849465</v>
+        <v>0.2607140148598601</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2055</v>
+        <v>15649</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.957336676120758</v>
+        <v>0.918267160654068</v>
       </c>
       <c r="D97" t="n">
-        <v>0.2554491550175972</v>
+        <v>0.2606519103572184</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1540</v>
+        <v>13204</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9584562381108602</v>
+        <v>0.9182976722717285</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2553031261409769</v>
+        <v>0.2606477645400461</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2605</v>
+        <v>16128</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9584562381108602</v>
+        <v>0.9185062646865845</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2553031261409769</v>
+        <v>0.2606194252285552</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>4140</v>
+        <v>16348</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.958456406990687</v>
+        <v>0.9185771703720093</v>
       </c>
       <c r="D100" t="n">
-        <v>0.2553031041259106</v>
+        <v>0.2606097934038539</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>5205</v>
+        <v>23651</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0.958456406990687</v>
+        <v>0.9187114040056864</v>
       </c>
       <c r="D101" t="n">
-        <v>0.2553031041259106</v>
+        <v>0.2605915610634054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Files results run 2.
</commit_message>
<xml_diff>
--- a/output/support/scores.xlsx
+++ b/output/support/scores.xlsx
@@ -460,1399 +460,1399 @@
         <v>8798</v>
       </c>
       <c r="B2" t="n">
-        <v>24.8227</v>
+        <v>27.6439</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>12.41135</v>
+        <v>13.82195</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7038</v>
+        <v>39489</v>
       </c>
       <c r="B3" t="n">
-        <v>22.8009</v>
+        <v>27.6439</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>11.40045</v>
+        <v>13.82195</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3207</v>
+        <v>8050</v>
       </c>
       <c r="B4" t="n">
-        <v>22.8009</v>
+        <v>24.381</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>11.40045</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8050</v>
+        <v>33898</v>
       </c>
       <c r="B5" t="n">
-        <v>22.8009</v>
+        <v>24.381</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>11.40045</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9621</v>
+        <v>37729</v>
       </c>
       <c r="B6" t="n">
-        <v>22.8009</v>
+        <v>24.381</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>11.40045</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14202</v>
+        <v>7038</v>
       </c>
       <c r="B7" t="n">
-        <v>21.2276</v>
+        <v>24.381</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>10.6138</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6734</v>
+        <v>3207</v>
       </c>
       <c r="B8" t="n">
-        <v>21.2276</v>
+        <v>24.381</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>10.6138</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8731</v>
+        <v>9621</v>
       </c>
       <c r="B9" t="n">
-        <v>21.2276</v>
+        <v>24.381</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>10.6138</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1185</v>
+        <v>38741</v>
       </c>
       <c r="B10" t="n">
-        <v>21.2276</v>
+        <v>24.381</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>10.6138</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5216</v>
+        <v>40312</v>
       </c>
       <c r="B11" t="n">
-        <v>19.8573</v>
+        <v>24.381</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>9.928649999999999</v>
+        <v>12.1905</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>21168</v>
+        <v>39422</v>
       </c>
       <c r="B12" t="n">
-        <v>19.8573</v>
+        <v>23.1997</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>9.928649999999999</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1408</v>
+        <v>31876</v>
       </c>
       <c r="B13" t="n">
-        <v>19.8573</v>
+        <v>23.1997</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>9.928649999999999</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2924</v>
+        <v>44893</v>
       </c>
       <c r="B14" t="n">
-        <v>18.6533</v>
+        <v>23.1997</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>9.326650000000001</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2909</v>
+        <v>1185</v>
       </c>
       <c r="B15" t="n">
-        <v>18.6533</v>
+        <v>23.1997</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>9.326650000000001</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7485</v>
+        <v>6734</v>
       </c>
       <c r="B16" t="n">
-        <v>18.6533</v>
+        <v>23.1997</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>9.326650000000001</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1506</v>
+        <v>14202</v>
       </c>
       <c r="B17" t="n">
-        <v>18.6533</v>
+        <v>23.1997</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>9.326650000000001</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>781</v>
+        <v>37425</v>
       </c>
       <c r="B18" t="n">
-        <v>16.80278333333333</v>
+        <v>23.1997</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>8.401391666666667</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3152</v>
+        <v>8731</v>
       </c>
       <c r="B19" t="n">
-        <v>15.9631</v>
+        <v>23.1997</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>7.981550000000001</v>
+        <v>11.59985</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10197</v>
+        <v>21168</v>
       </c>
       <c r="B20" t="n">
-        <v>15.9631</v>
+        <v>22.1277</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>7.981550000000001</v>
+        <v>11.06385</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>21975</v>
+        <v>35907</v>
       </c>
       <c r="B21" t="n">
-        <v>15.9225</v>
+        <v>22.1277</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>7.96125</v>
+        <v>11.06385</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>23121</v>
+        <v>1408</v>
       </c>
       <c r="B22" t="n">
-        <v>15.9225</v>
+        <v>22.1277</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>7.96125</v>
+        <v>11.06385</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>21098</v>
+        <v>32099</v>
       </c>
       <c r="B23" t="n">
-        <v>15.3925</v>
+        <v>22.1277</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>7.69625</v>
+        <v>11.06385</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>12690</v>
+        <v>51859</v>
       </c>
       <c r="B24" t="n">
-        <v>14.7781</v>
+        <v>22.1277</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>7.38905</v>
+        <v>11.06385</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1008</v>
+        <v>5216</v>
       </c>
       <c r="B25" t="n">
-        <v>14.2776</v>
+        <v>22.1277</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>7.1388</v>
+        <v>11.06385</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>18794</v>
+        <v>32197</v>
       </c>
       <c r="B26" t="n">
-        <v>13.8833</v>
+        <v>21.1503</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6.94165</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>7961</v>
+        <v>7485</v>
       </c>
       <c r="B27" t="n">
-        <v>13.8833</v>
+        <v>21.1503</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6.94165</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>22045</v>
+        <v>33600</v>
       </c>
       <c r="B28" t="n">
-        <v>13.5616</v>
+        <v>21.1503</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6.7808</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3376</v>
+        <v>2924</v>
       </c>
       <c r="B29" t="n">
-        <v>13.5616</v>
+        <v>21.1503</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6.7808</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>16730</v>
+        <v>38176</v>
       </c>
       <c r="B30" t="n">
-        <v>13.5616</v>
+        <v>21.1503</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6.7808</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4930</v>
+        <v>1506</v>
       </c>
       <c r="B31" t="n">
-        <v>13.5428</v>
+        <v>21.1503</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>6.7714</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7168</v>
+        <v>2909</v>
       </c>
       <c r="B32" t="n">
-        <v>13.3676</v>
+        <v>21.1503</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6.6838</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7930</v>
+        <v>33615</v>
       </c>
       <c r="B33" t="n">
-        <v>13.0587</v>
+        <v>21.1503</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>6.52935</v>
+        <v>10.57515</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>9114</v>
+        <v>781</v>
       </c>
       <c r="B34" t="n">
-        <v>12.8873</v>
+        <v>20.35443333333333</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>6.443650000000001</v>
+        <v>10.17721666666667</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9525</v>
+        <v>31472</v>
       </c>
       <c r="B35" t="n">
-        <v>12.8873</v>
+        <v>20.35443333333333</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>6.443650000000001</v>
+        <v>10.17721666666667</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4168</v>
+        <v>3152</v>
       </c>
       <c r="B36" t="n">
-        <v>12.8873</v>
+        <v>18.2692</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>6.443650000000001</v>
+        <v>9.134600000000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>25631</v>
+        <v>33843</v>
       </c>
       <c r="B37" t="n">
-        <v>12.8873</v>
+        <v>18.2692</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6.443650000000001</v>
+        <v>9.134600000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>383</v>
+        <v>63057</v>
       </c>
       <c r="B38" t="n">
-        <v>12.8873</v>
+        <v>17.8789</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6.443650000000001</v>
+        <v>8.939450000000001</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>17024</v>
+        <v>49485</v>
       </c>
       <c r="B39" t="n">
-        <v>12.8873</v>
+        <v>17.4886</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>6.443650000000001</v>
+        <v>8.744300000000001</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>14626</v>
+        <v>38652</v>
       </c>
       <c r="B40" t="n">
-        <v>12.8873</v>
+        <v>17.4886</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.443650000000001</v>
+        <v>8.744300000000001</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>11980</v>
+        <v>18794</v>
       </c>
       <c r="B41" t="n">
-        <v>12.8873</v>
+        <v>17.4886</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6.443650000000001</v>
+        <v>8.744300000000001</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>7995</v>
+        <v>7961</v>
       </c>
       <c r="B42" t="n">
-        <v>12.8873</v>
+        <v>17.4886</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>6.443650000000001</v>
+        <v>8.744300000000001</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>21226</v>
+        <v>10197</v>
       </c>
       <c r="B43" t="n">
-        <v>12.8873</v>
+        <v>17.2113</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6.443650000000001</v>
+        <v>8.605650000000001</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>9700</v>
+        <v>40888</v>
       </c>
       <c r="B44" t="n">
-        <v>12.8873</v>
+        <v>17.2113</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>6.443650000000001</v>
+        <v>8.605650000000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>19467</v>
+        <v>21975</v>
       </c>
       <c r="B45" t="n">
-        <v>12.8873</v>
+        <v>17.196</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6.443650000000001</v>
+        <v>8.598000000000001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>17046</v>
+        <v>23121</v>
       </c>
       <c r="B46" t="n">
-        <v>12.8725</v>
+        <v>17.196</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6.43625</v>
+        <v>8.598000000000001</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>13856</v>
+        <v>52666</v>
       </c>
       <c r="B47" t="n">
-        <v>12.2241</v>
+        <v>17.196</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6.11205</v>
+        <v>8.598000000000001</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>13374</v>
+        <v>53812</v>
       </c>
       <c r="B48" t="n">
-        <v>12.2241</v>
+        <v>17.196</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6.11205</v>
+        <v>8.598000000000001</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>21436</v>
+        <v>1008</v>
       </c>
       <c r="B49" t="n">
-        <v>12.091</v>
+        <v>17.0331</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6.0455</v>
+        <v>8.516550000000001</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2848</v>
+        <v>31699</v>
       </c>
       <c r="B50" t="n">
-        <v>12.091</v>
+        <v>17.0331</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.0455</v>
+        <v>8.516550000000001</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>18275</v>
+        <v>7168</v>
       </c>
       <c r="B51" t="n">
-        <v>12.0605</v>
+        <v>16.7464</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6.03025</v>
+        <v>8.373200000000001</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>12094</v>
+        <v>62745</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8988950252532959</v>
+        <v>0.927051842212677</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2633110273872588</v>
+        <v>0.2594636994435451</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>315</v>
+        <v>48068</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8995209634304047</v>
+        <v>0.9287070035934448</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2632242600245034</v>
+        <v>0.2592410350916088</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>15965</v>
+        <v>41948</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9020004272460938</v>
+        <v>0.9291778802871704</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2628811186567134</v>
+        <v>0.2591777591424446</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>18097</v>
+        <v>52478</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9020424783229828</v>
+        <v>0.9304040670394897</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2628753067811853</v>
+        <v>0.259013130223462</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1974</v>
+        <v>46340</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.9023942947387695</v>
+        <v>0.9315143823623657</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2628266923333358</v>
+        <v>0.2588642386335576</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>12756</v>
+        <v>44100</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9029656648635864</v>
+        <v>0.9330952763557434</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2627477779720436</v>
+        <v>0.2586525382973343</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>17243</v>
+        <v>62682</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9031985998153687</v>
+        <v>0.9349758625030518</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2627156199297885</v>
+        <v>0.2584011561535494</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>14790</v>
+        <v>41237</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9039535522460938</v>
+        <v>0.935991644859314</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2626114483781131</v>
+        <v>0.2582655773993975</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>11250</v>
+        <v>41947</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9044677019119263</v>
+        <v>0.9366505146026611</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2625405510936425</v>
+        <v>0.2581777126176966</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>5203</v>
+        <v>41215</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9044732451438904</v>
+        <v>0.9389761686325073</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2625397869331701</v>
+        <v>0.2578680481424548</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>10539</v>
+        <v>47400</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.905234232544899</v>
+        <v>0.9391109943389893</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2624349234645704</v>
+        <v>0.2578501186676226</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>11860</v>
+        <v>61528</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9052505493164062</v>
+        <v>0.9414780288934708</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2624326759435379</v>
+        <v>0.2575357498559852</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>14704</v>
+        <v>61790</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9056225717067719</v>
+        <v>0.9417414466540018</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2623814429067004</v>
+        <v>0.2575008124081593</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>17269</v>
+        <v>42703</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.906856432557106</v>
+        <v>0.9428327679634094</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2622116649492574</v>
+        <v>0.2573561699415484</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>13147</v>
+        <v>34233</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9072015881538391</v>
+        <v>0.9430048942565918</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2621642112221589</v>
+        <v>0.2573333713558677</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>4455</v>
+        <v>30800</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9072189182043076</v>
+        <v>0.9434165358543396</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2621618290525148</v>
+        <v>0.25727886470833</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>26999</v>
+        <v>61749</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9076013565063477</v>
+        <v>0.9435157775878906</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2621092705216559</v>
+        <v>0.2572657272793293</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>5226</v>
+        <v>63516</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.9076150059700012</v>
+        <v>0.9436931014060974</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2621073950641081</v>
+        <v>0.2572422568348328</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>14251</v>
+        <v>63448</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.9079282283782959</v>
+        <v>0.9443814754486084</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2620643651910276</v>
+        <v>0.2571511847409675</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>13100</v>
+        <v>62645</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9079800844192505</v>
+        <v>0.9447107911109924</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2620572426740972</v>
+        <v>0.2571076389792414</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>3085</v>
+        <v>63549</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9084427356719971</v>
+        <v>0.9447325269381205</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2619937138558894</v>
+        <v>0.2571047653464324</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>13442</v>
+        <v>46320</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.908580482006073</v>
+        <v>0.9447975953420004</v>
       </c>
       <c r="D73" t="n">
-        <v>0.261974805209398</v>
+        <v>0.2570961632190176</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>16205</v>
+        <v>63680</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9086835086345673</v>
+        <v>0.9451080560684204</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2619606643731572</v>
+        <v>0.2570551278321435</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>21782</v>
+        <v>63783</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9090400040149689</v>
+        <v>0.945293977856636</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2619117456671586</v>
+        <v>0.2570305597465068</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>14463</v>
+        <v>62366</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9099763184785843</v>
+        <v>0.9455844163894653</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2617833504858748</v>
+        <v>0.2569921900011304</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>4653</v>
+        <v>42895</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9101221164067587</v>
+        <v>0.9460306763648987</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2617633687947548</v>
+        <v>0.2569332570512087</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>13638</v>
+        <v>62554</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9104804793993632</v>
+        <v>0.9461007714271545</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2617142678983013</v>
+        <v>0.2569240027757297</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>15886</v>
+        <v>62031</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9106599092483521</v>
+        <v>0.9462374329566956</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2616896903419607</v>
+        <v>0.2569059620030056</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>4961</v>
+        <v>62555</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9115528225898742</v>
+        <v>0.9462606757879257</v>
       </c>
       <c r="D80" t="n">
-        <v>0.2615674513888521</v>
+        <v>0.2569028939546238</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>5114</v>
+        <v>62777</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9117672840754191</v>
+        <v>0.946341872215271</v>
       </c>
       <c r="D81" t="n">
-        <v>0.2615381088299213</v>
+        <v>0.2568921766199862</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>17377</v>
+        <v>48030</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9118037819862366</v>
+        <v>0.9465028444925944</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2615331158517394</v>
+        <v>0.2568709320999414</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>11873</v>
+        <v>63713</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9126194715499878</v>
+        <v>0.9466245532035827</v>
       </c>
       <c r="D83" t="n">
-        <v>0.2614215778085746</v>
+        <v>0.2568548717713152</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>16130</v>
+        <v>63118</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.9132238427797953</v>
+        <v>0.9468721747398376</v>
       </c>
       <c r="D84" t="n">
-        <v>0.2613389969432595</v>
+        <v>0.2568222025500033</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1968</v>
+        <v>62302</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9138243198394775</v>
+        <v>0.9469994306564331</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2612569998284574</v>
+        <v>0.2568054166463852</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>29079</v>
+        <v>44916</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9138715147972107</v>
+        <v>0.9473431706428528</v>
       </c>
       <c r="D86" t="n">
-        <v>0.2612505573828862</v>
+        <v>0.256760086017577</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>7855</v>
+        <v>63415</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9144208331902822</v>
+        <v>0.9474191665649414</v>
       </c>
       <c r="D87" t="n">
-        <v>0.2611755949013447</v>
+        <v>0.2567500662335328</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>10524</v>
+        <v>32912</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9147552102804184</v>
+        <v>0.9478703737258911</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2611299853451107</v>
+        <v>0.2566905923229372</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>13384</v>
+        <v>47913</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9150511920452118</v>
+        <v>0.9480764120817184</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2610896262600774</v>
+        <v>0.2566634434353111</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>17256</v>
+        <v>61807</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9152307748794556</v>
+        <v>0.9481077790260315</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2610651450248704</v>
+        <v>0.2566593108364765</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>13990</v>
+        <v>61864</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9154833257198334</v>
+        <v>0.9481930136680603</v>
       </c>
       <c r="D91" t="n">
-        <v>0.261030724353657</v>
+        <v>0.2566480818338422</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>13782</v>
+        <v>63049</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9158063769340515</v>
+        <v>0.9490892191727957</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2609867082706823</v>
+        <v>0.2565300731652514</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>15737</v>
+        <v>61865</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9161118268966675</v>
+        <v>0.9497653603553772</v>
       </c>
       <c r="D93" t="n">
-        <v>0.2609451040286095</v>
+        <v>0.2564411134624254</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>12204</v>
+        <v>62589</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9174277037382126</v>
+        <v>0.9498928785324097</v>
       </c>
       <c r="D94" t="n">
-        <v>0.2607660247242705</v>
+        <v>0.2564243428471444</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>15638</v>
+        <v>63099</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.917534863948822</v>
+        <v>0.9499646425247192</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2607514519816025</v>
+        <v>0.2564149057352262</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>11256</v>
+        <v>61431</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9178102115790049</v>
+        <v>0.9501596689224243</v>
       </c>
       <c r="D96" t="n">
-        <v>0.2607140148598601</v>
+        <v>0.2563892628731671</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>15649</v>
+        <v>61653</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.918267160654068</v>
+        <v>0.9502450704574585</v>
       </c>
       <c r="D97" t="n">
-        <v>0.2606519103572184</v>
+        <v>0.2563780355474595</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>13204</v>
+        <v>62049</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9182976722717285</v>
+        <v>0.9506577610969543</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2606477645400461</v>
+        <v>0.25632379496382</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>16128</v>
+        <v>63447</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9185062646865845</v>
+        <v>0.950806051492691</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2606194252285552</v>
+        <v>0.2563043105271366</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>16348</v>
+        <v>63437</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9185771703720093</v>
+        <v>0.9523679812749227</v>
       </c>
       <c r="D100" t="n">
-        <v>0.2606097934038539</v>
+        <v>0.2560992624318154</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>23651</v>
+        <v>61809</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0.9187114040056864</v>
+        <v>0.9531015753746033</v>
       </c>
       <c r="D101" t="n">
-        <v>0.2605915610634054</v>
+        <v>0.256003070349324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chunking output using punkt
</commit_message>
<xml_diff>
--- a/output/support/scores.xlsx
+++ b/output/support/scores.xlsx
@@ -457,1402 +457,1402 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8798</v>
+        <v>8669</v>
       </c>
       <c r="B2" t="n">
-        <v>24.8227</v>
+        <v>28.6202</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>12.41135</v>
+        <v>14.3101</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7038</v>
+        <v>3078</v>
       </c>
       <c r="B3" t="n">
-        <v>22.8009</v>
+        <v>24.7669</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>11.40045</v>
+        <v>12.38345</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3207</v>
+        <v>6909</v>
       </c>
       <c r="B4" t="n">
-        <v>22.8009</v>
+        <v>24.7669</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>11.40045</v>
+        <v>12.38345</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8050</v>
+        <v>9492</v>
       </c>
       <c r="B5" t="n">
-        <v>22.8009</v>
+        <v>24.7669</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>11.40045</v>
+        <v>12.38345</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9621</v>
+        <v>7921</v>
       </c>
       <c r="B6" t="n">
-        <v>22.8009</v>
+        <v>24.7669</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>11.40045</v>
+        <v>12.38345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14202</v>
+        <v>8602</v>
       </c>
       <c r="B7" t="n">
-        <v>21.2276</v>
+        <v>23.8251</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>10.6138</v>
+        <v>11.91255</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6734</v>
+        <v>14073</v>
       </c>
       <c r="B8" t="n">
-        <v>21.2276</v>
+        <v>23.8251</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>10.6138</v>
+        <v>11.91255</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8731</v>
+        <v>6605</v>
       </c>
       <c r="B9" t="n">
-        <v>21.2276</v>
+        <v>23.8251</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>10.6138</v>
+        <v>11.91255</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1185</v>
+        <v>1056</v>
       </c>
       <c r="B10" t="n">
-        <v>21.2276</v>
+        <v>23.8251</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>10.6138</v>
+        <v>11.91255</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5216</v>
+        <v>1279</v>
       </c>
       <c r="B11" t="n">
-        <v>19.8573</v>
+        <v>22.9522</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>9.928649999999999</v>
+        <v>11.4761</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>21168</v>
+        <v>5087</v>
       </c>
       <c r="B12" t="n">
-        <v>19.8573</v>
+        <v>22.9522</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>9.928649999999999</v>
+        <v>11.4761</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1408</v>
+        <v>21039</v>
       </c>
       <c r="B13" t="n">
-        <v>19.8573</v>
+        <v>22.9522</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>9.928649999999999</v>
+        <v>11.4761</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2924</v>
+        <v>1377</v>
       </c>
       <c r="B14" t="n">
-        <v>18.6533</v>
+        <v>22.1411</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>9.326650000000001</v>
+        <v>11.07055</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2909</v>
+        <v>2795</v>
       </c>
       <c r="B15" t="n">
-        <v>18.6533</v>
+        <v>22.1411</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>9.326650000000001</v>
+        <v>11.07055</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7485</v>
+        <v>7356</v>
       </c>
       <c r="B16" t="n">
-        <v>18.6533</v>
+        <v>22.1411</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>9.326650000000001</v>
+        <v>11.07055</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1506</v>
+        <v>2780</v>
       </c>
       <c r="B17" t="n">
-        <v>18.6533</v>
+        <v>22.1411</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>9.326650000000001</v>
+        <v>11.07055</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>781</v>
+        <v>652</v>
       </c>
       <c r="B18" t="n">
-        <v>16.80278333333333</v>
+        <v>21.57673333333333</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>8.401391666666667</v>
+        <v>10.78836666666667</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3152</v>
+        <v>31828</v>
       </c>
       <c r="B19" t="n">
-        <v>15.9631</v>
+        <v>20.7024</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>7.981550000000001</v>
+        <v>10.3512</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10197</v>
+        <v>7832</v>
       </c>
       <c r="B20" t="n">
-        <v>15.9631</v>
+        <v>18.8674</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>7.981550000000001</v>
+        <v>9.4337</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>21975</v>
+        <v>18665</v>
       </c>
       <c r="B21" t="n">
-        <v>15.9225</v>
+        <v>18.8674</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>7.96125</v>
+        <v>9.4337</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>23121</v>
+        <v>3023</v>
       </c>
       <c r="B22" t="n">
-        <v>15.9225</v>
+        <v>18.815</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>7.96125</v>
+        <v>9.407500000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>21098</v>
+        <v>7039</v>
       </c>
       <c r="B23" t="n">
-        <v>15.3925</v>
+        <v>18.1589</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>7.69625</v>
+        <v>9.07945</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>12690</v>
+        <v>879</v>
       </c>
       <c r="B24" t="n">
-        <v>14.7781</v>
+        <v>17.8582</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>7.38905</v>
+        <v>8.9291</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1008</v>
+        <v>21307</v>
       </c>
       <c r="B25" t="n">
-        <v>14.2776</v>
+        <v>17.485</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>7.1388</v>
+        <v>8.7425</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>18794</v>
+        <v>2719</v>
       </c>
       <c r="B26" t="n">
-        <v>13.8833</v>
+        <v>17.485</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6.94165</v>
+        <v>8.7425</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>7961</v>
+        <v>3247</v>
       </c>
       <c r="B27" t="n">
-        <v>13.8833</v>
+        <v>17.4154</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6.94165</v>
+        <v>8.707700000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>22045</v>
+        <v>21916</v>
       </c>
       <c r="B28" t="n">
-        <v>13.5616</v>
+        <v>17.4154</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6.7808</v>
+        <v>8.707700000000001</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>3376</v>
+        <v>21846</v>
       </c>
       <c r="B29" t="n">
-        <v>13.5616</v>
+        <v>17.3028</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>6.7808</v>
+        <v>8.651400000000001</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>16730</v>
+        <v>22992</v>
       </c>
       <c r="B30" t="n">
-        <v>13.5616</v>
+        <v>17.3028</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>6.7808</v>
+        <v>8.651400000000001</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>4930</v>
+        <v>10068</v>
       </c>
       <c r="B31" t="n">
-        <v>13.5428</v>
+        <v>17.2222</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>6.7714</v>
+        <v>8.6111</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>7168</v>
+        <v>4801</v>
       </c>
       <c r="B32" t="n">
-        <v>13.3676</v>
+        <v>16.9468</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>6.6838</v>
+        <v>8.4734</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>7930</v>
+        <v>16601</v>
       </c>
       <c r="B33" t="n">
-        <v>13.0587</v>
+        <v>15.9411</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>6.52935</v>
+        <v>7.97055</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>9114</v>
+        <v>4039</v>
       </c>
       <c r="B34" t="n">
-        <v>12.8873</v>
+        <v>15.7507</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>6.443650000000001</v>
+        <v>7.87535</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9525</v>
+        <v>8985</v>
       </c>
       <c r="B35" t="n">
-        <v>12.8873</v>
+        <v>15.7507</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>6.443650000000001</v>
+        <v>7.87535</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4168</v>
+        <v>21097</v>
       </c>
       <c r="B36" t="n">
-        <v>12.8873</v>
+        <v>15.7507</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>6.443650000000001</v>
+        <v>7.87535</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>25631</v>
+        <v>19338</v>
       </c>
       <c r="B37" t="n">
-        <v>12.8873</v>
+        <v>15.7507</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>6.443650000000001</v>
+        <v>7.87535</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>383</v>
+        <v>7866</v>
       </c>
       <c r="B38" t="n">
-        <v>12.8873</v>
+        <v>15.7507</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>6.443650000000001</v>
+        <v>7.87535</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>17024</v>
+        <v>14497</v>
       </c>
       <c r="B39" t="n">
-        <v>12.8873</v>
+        <v>15.7507</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>6.443650000000001</v>
+        <v>7.87535</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>14626</v>
+        <v>20969</v>
       </c>
       <c r="B40" t="n">
-        <v>12.8873</v>
+        <v>15.168</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>6.443650000000001</v>
+        <v>7.584</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>11980</v>
+        <v>13536</v>
       </c>
       <c r="B41" t="n">
-        <v>12.8873</v>
+        <v>15.0746</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>6.443650000000001</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>7995</v>
+        <v>7269</v>
       </c>
       <c r="B42" t="n">
-        <v>12.8873</v>
+        <v>15.0746</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>6.443650000000001</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>21226</v>
+        <v>8033</v>
       </c>
       <c r="B43" t="n">
-        <v>12.8873</v>
+        <v>15.0746</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>6.443650000000001</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>9700</v>
+        <v>14667</v>
       </c>
       <c r="B44" t="n">
-        <v>12.8873</v>
+        <v>15.0746</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>6.443650000000001</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>19467</v>
+        <v>5426</v>
       </c>
       <c r="B45" t="n">
-        <v>12.8873</v>
+        <v>15.0746</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>6.443650000000001</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>17046</v>
+        <v>5379</v>
       </c>
       <c r="B46" t="n">
-        <v>12.8725</v>
+        <v>15.0746</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>6.43625</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>13856</v>
+        <v>974</v>
       </c>
       <c r="B47" t="n">
-        <v>12.2241</v>
+        <v>15.0746</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>6.11205</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>13374</v>
+        <v>19576</v>
       </c>
       <c r="B48" t="n">
-        <v>12.2241</v>
+        <v>15.0746</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>6.11205</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>21436</v>
+        <v>5373</v>
       </c>
       <c r="B49" t="n">
-        <v>12.091</v>
+        <v>15.0746</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>6.0455</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2848</v>
+        <v>19416</v>
       </c>
       <c r="B50" t="n">
-        <v>12.091</v>
+        <v>15.0746</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>6.0455</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>18275</v>
+        <v>8055</v>
       </c>
       <c r="B51" t="n">
-        <v>12.0605</v>
+        <v>15.0746</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>6.03025</v>
+        <v>7.5373</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>12094</v>
+        <v>32598</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8988950252532959</v>
+        <v>0.927051842212677</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2633110273872588</v>
+        <v>0.2594636994435451</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>315</v>
+        <v>17248</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8995209634304047</v>
+        <v>0.9287068843841553</v>
       </c>
       <c r="D53" t="n">
-        <v>0.2632242600245034</v>
+        <v>0.2592410511147484</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>15965</v>
+        <v>11128</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0.9020004272460938</v>
+        <v>0.9291775226593018</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2628811186567134</v>
+        <v>0.2591778071884064</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>18097</v>
+        <v>21658</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9020424783229828</v>
+        <v>0.9304042458534241</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2628753067811853</v>
+        <v>0.2590131062309967</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1974</v>
+        <v>15520</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>0.9023942947387695</v>
+        <v>0.9315145015716553</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2628266923333358</v>
+        <v>0.2588642226569641</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>12756</v>
+        <v>13280</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>0.9029656648635864</v>
+        <v>0.9330949783325195</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2627477779720436</v>
+        <v>0.2586525781735247</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>17243</v>
+        <v>33206</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>0.9031985998153687</v>
+        <v>0.9349755048751831</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2627156199297885</v>
+        <v>0.2584012039120117</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>14790</v>
+        <v>10417</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>0.9039535522460938</v>
+        <v>0.9359915852546692</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2626114483781131</v>
+        <v>0.2582655853507895</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>11250</v>
+        <v>11127</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9044677019119263</v>
+        <v>0.9366506934165955</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2625405510936425</v>
+        <v>0.2581776887797517</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>5203</v>
+        <v>32546</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9044732451438904</v>
+        <v>0.9368192553520203</v>
       </c>
       <c r="D61" t="n">
-        <v>0.2625397869331701</v>
+        <v>0.2581552195014316</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>10539</v>
+        <v>16580</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>0.905234232544899</v>
+        <v>0.9386512637138367</v>
       </c>
       <c r="D62" t="n">
-        <v>0.2624349234645704</v>
+        <v>0.2579112650937331</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>11860</v>
+        <v>10395</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9052505493164062</v>
+        <v>0.9389759302139282</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2624326759435379</v>
+        <v>0.2578680798501891</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>14704</v>
+        <v>3413</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>0.9056225717067719</v>
+        <v>0.9399219393730164</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2623814429067004</v>
+        <v>0.2577423296535325</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>17269</v>
+        <v>30671</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>0.906856432557106</v>
+        <v>0.9407529354095459</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2622116649492574</v>
+        <v>0.2576319689525488</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>13147</v>
+        <v>32910</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>0.9072015881538391</v>
+        <v>0.9416920244693756</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2621642112221589</v>
+        <v>0.2575073666157947</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>4455</v>
+        <v>17210</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9072189182043076</v>
+        <v>0.9421557039022446</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2621618290525148</v>
+        <v>0.2574458880899112</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>26999</v>
+        <v>32214</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9076013565063477</v>
+        <v>0.9423157811164856</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2621092705216559</v>
+        <v>0.2574246705201505</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>5226</v>
+        <v>30957</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>0.9076150059700012</v>
+        <v>0.9425412058830261</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2621073950641081</v>
+        <v>0.2573947973333794</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>14251</v>
+        <v>31782</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0.9079282283782959</v>
+        <v>0.9430217742919922</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2620643651910276</v>
+        <v>0.257331135767736</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>13100</v>
+        <v>32492</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0.9079800844192505</v>
+        <v>0.9436438202857971</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2620572426740972</v>
+        <v>0.2572487792163891</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>3085</v>
+        <v>32764</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0.9084427356719971</v>
+        <v>0.9436925649642944</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2619937138558894</v>
+        <v>0.2572423278314001</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>13442</v>
+        <v>31274</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>0.908580482006073</v>
+        <v>0.9437344312667847</v>
       </c>
       <c r="D73" t="n">
-        <v>0.261974805209398</v>
+        <v>0.2572367870615619</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>16205</v>
+        <v>32304</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9086835086345673</v>
+        <v>0.9437475800514221</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2619606643731572</v>
+        <v>0.2572350469430668</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>21782</v>
+        <v>32491</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9090400040149689</v>
+        <v>0.9440440436204275</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2619117456671586</v>
+        <v>0.2571958190149032</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>14463</v>
+        <v>11883</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9099763184785843</v>
+        <v>0.9441129366556803</v>
       </c>
       <c r="D76" t="n">
-        <v>0.2617833504858748</v>
+        <v>0.2571867048321352</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>4653</v>
+        <v>33169</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0.9101221164067587</v>
+        <v>0.944710373878479</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2617633687947548</v>
+        <v>0.2571076941410114</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>13638</v>
+        <v>15500</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>0.9104804793993632</v>
+        <v>0.9450543721516927</v>
       </c>
       <c r="D78" t="n">
-        <v>0.2617142678983013</v>
+        <v>0.257062222608657</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>15886</v>
+        <v>14096</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>0.9106599092483521</v>
+        <v>0.9451887249946594</v>
       </c>
       <c r="D79" t="n">
-        <v>0.2616896903419607</v>
+        <v>0.257044467498326</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>4961</v>
+        <v>31275</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>0.9115528225898742</v>
+        <v>0.9452362179756164</v>
       </c>
       <c r="D80" t="n">
-        <v>0.2615674513888521</v>
+        <v>0.2570381917525389</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>5114</v>
+        <v>12075</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9117672840754191</v>
+        <v>0.9460304975509644</v>
       </c>
       <c r="D81" t="n">
-        <v>0.2615381088299213</v>
+        <v>0.2569332806599068</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>17377</v>
+        <v>31424</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9118037819862366</v>
+        <v>0.9460898737112681</v>
       </c>
       <c r="D82" t="n">
-        <v>0.2615331158517394</v>
+        <v>0.2569254414989997</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>11873</v>
+        <v>31141</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>0.9126194715499878</v>
+        <v>0.9468664824962616</v>
       </c>
       <c r="D83" t="n">
-        <v>0.2614215778085746</v>
+        <v>0.2568229534461463</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>16130</v>
+        <v>32196</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>0.9132238427797953</v>
+        <v>0.9474999904632568</v>
       </c>
       <c r="D84" t="n">
-        <v>0.2613389969432595</v>
+        <v>0.2567394107565894</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1968</v>
+        <v>31537</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
       </c>
       <c r="C85" t="n">
-        <v>0.9138243198394775</v>
+        <v>0.9478140950202942</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2612569998284574</v>
+        <v>0.2566980089518197</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>29079</v>
+        <v>31217</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
       </c>
       <c r="C86" t="n">
-        <v>0.9138715147972107</v>
+        <v>0.9478141665458679</v>
       </c>
       <c r="D86" t="n">
-        <v>0.2612505573828862</v>
+        <v>0.2566979995256266</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>7855</v>
+        <v>31108</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
       </c>
       <c r="C87" t="n">
-        <v>0.9144208331902822</v>
+        <v>0.9478356242179871</v>
       </c>
       <c r="D87" t="n">
-        <v>0.2611755949013447</v>
+        <v>0.2566951716989666</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>10524</v>
+        <v>31820</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9147552102804184</v>
+        <v>0.9484389623006185</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2611299853451107</v>
+        <v>0.2566156855176131</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>13384</v>
+        <v>33113</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>0.9150511920452118</v>
+        <v>0.9508030116558075</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2610896262600774</v>
+        <v>0.2563047099130777</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>17256</v>
+        <v>17093</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9152307748794556</v>
+        <v>0.9509496688842773</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2610651450248704</v>
+        <v>0.2562854429176246</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>13990</v>
+        <v>31879</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
       </c>
       <c r="C91" t="n">
-        <v>0.9154833257198334</v>
+        <v>0.9513483881950379</v>
       </c>
       <c r="D91" t="n">
-        <v>0.261030724353657</v>
+        <v>0.2562330760743811</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>13782</v>
+        <v>30959</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
       </c>
       <c r="C92" t="n">
-        <v>0.9158063769340515</v>
+        <v>0.9515502214431762</v>
       </c>
       <c r="D92" t="n">
-        <v>0.2609867082706823</v>
+        <v>0.2562065759344122</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>15737</v>
+        <v>31414</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>0.9161118268966675</v>
+        <v>0.95162100593249</v>
       </c>
       <c r="D93" t="n">
-        <v>0.2609451040286095</v>
+        <v>0.2561972834275262</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>12204</v>
+        <v>33320</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0.9174277037382126</v>
+        <v>0.9526301324367523</v>
       </c>
       <c r="D94" t="n">
-        <v>0.2607660247242705</v>
+        <v>0.2560648797199669</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>15638</v>
+        <v>31810</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>0.917534863948822</v>
+        <v>0.9539956152439117</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2607514519816025</v>
+        <v>0.2558859375626523</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>11256</v>
+        <v>32913</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9178102115790049</v>
+        <v>0.9541786114374796</v>
       </c>
       <c r="D96" t="n">
-        <v>0.2607140148598601</v>
+        <v>0.2558619754988535</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>15649</v>
+        <v>31811</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
       </c>
       <c r="C97" t="n">
-        <v>0.918267160654068</v>
+        <v>0.9561859846115113</v>
       </c>
       <c r="D97" t="n">
-        <v>0.2606519103572184</v>
+        <v>0.2555994184261051</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>13204</v>
+        <v>32842</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0.9182976722717285</v>
+        <v>0.9562437534332275</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2606477645400461</v>
+        <v>0.2555918704519797</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>16128</v>
+        <v>32056</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
       </c>
       <c r="C99" t="n">
-        <v>0.9185062646865845</v>
+        <v>0.9564313193162283</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2606194252285552</v>
+        <v>0.2555673664919399</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>16348</v>
+        <v>32964</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
       </c>
       <c r="C100" t="n">
-        <v>0.9185771703720093</v>
+        <v>0.9564313193162283</v>
       </c>
       <c r="D100" t="n">
-        <v>0.2606097934038539</v>
+        <v>0.2555673664919399</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>23651</v>
+        <v>12255</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
       </c>
       <c r="C101" t="n">
-        <v>0.9187114040056864</v>
+        <v>0.9572775363922119</v>
       </c>
       <c r="D101" t="n">
-        <v>0.2605915610634054</v>
+        <v>0.2554568734905293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>